<commit_message>
#2279 - Ajustes CheckList da Qualidade - GCO
</commit_message>
<xml_diff>
--- a/Doc-DD-UFG/Qualidade/Gerência/checklist_qualidade_GCO-1.0.0_SDD-UFG.xlsx
+++ b/Doc-DD-UFG/Qualidade/Gerência/checklist_qualidade_GCO-1.0.0_SDD-UFG.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Nº</t>
   </si>
@@ -84,19 +84,22 @@
     <t>Evidencia 2</t>
   </si>
   <si>
-    <t>Não foram criadas baselines</t>
-  </si>
-  <si>
     <t>Não</t>
   </si>
   <si>
-    <t>Ainda não foram feitas auditorias, pois ainda não existe baseline.</t>
-  </si>
-  <si>
-    <t>Não existem documentos do processo GCO no repositório além do Plano de Configuração.</t>
-  </si>
-  <si>
     <t>O Plano de Configuração não foi aprovado.</t>
+  </si>
+  <si>
+    <t>O Plano de Projeto não está disponível no Repositório. O Plano de Configuração não foi aprovado.</t>
+  </si>
+  <si>
+    <t>Não existem documentos do processo GCO no repositório além do Plano de Configuração. O Plano de Projeto não está disponível no repositório para verificação dos artefatos que devem ser entregues pela GCO e o Plano de Configuração não contempla essa informação.</t>
+  </si>
+  <si>
+    <t>Ainda não foram feitas auditorias, pois ainda não existem baselines.</t>
+  </si>
+  <si>
+    <t>O Plano de Projeto não está no repositório para verificação de planejamento de baselines. Não foram criadas baselines.</t>
   </si>
 </sst>
 </file>
@@ -176,13 +179,23 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -467,16 +480,16 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="133.140625" customWidth="1"/>
+    <col min="2" max="2" width="60.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="76.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -499,7 +512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -519,7 +532,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -536,7 +549,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -553,7 +566,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -566,10 +579,10 @@
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -586,7 +599,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -603,7 +616,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -620,7 +633,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -633,10 +646,10 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -644,7 +657,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -652,7 +665,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -672,7 +685,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -689,7 +702,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -702,10 +715,10 @@
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -713,11 +726,13 @@
         <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>

</xml_diff>